<commit_message>
Modified checklist for Iron team
</commit_message>
<xml_diff>
--- a/CheckList_IronIO.xlsx
+++ b/CheckList_IronIO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\МОиБД\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\МОиБД\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54277FA8-D53A-4044-841F-B2F180680D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202EFD11-FE83-4F5D-9DFB-FDE4E9316241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD5F888E-24C3-4E9C-A1DC-C3CCE5513399}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>№</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Дизайн</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Создание сессии</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Отзывчивость интерфейса</t>
   </si>
   <si>
-    <t>Все компоненты рабоатют быстро</t>
-  </si>
-  <si>
     <t>Скорость загрузки страниц</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>Функционал соответствует ТЗ, однако смена неинтуитивная.</t>
   </si>
   <si>
-    <t>Весь текст в программе соотвествует орфаграфическим нормам.</t>
-  </si>
-  <si>
     <t>Текст в программе довольно простой и понятный, однако многие поля и действия, которые необходимо совершить, непонятны. Необходимо дполнить программу полями с описанием или всплывающими окнами.</t>
   </si>
   <si>
@@ -166,6 +157,39 @@
   </si>
   <si>
     <t>При нажатии крестика, пользователя возвращает на окно входа.</t>
+  </si>
+  <si>
+    <t>Адаптивность интерфейса</t>
+  </si>
+  <si>
+    <t>Несмотря на работоспособность, при сжатии и расшерении теряется часть интерфейса. Резкие скачки элементов при сжатии.</t>
+  </si>
+  <si>
+    <t>Курсор</t>
+  </si>
+  <si>
+    <t>При использовании часто появляется каретка ввода, однако сам ввод не доступен или не поддерживается.</t>
+  </si>
+  <si>
+    <t>Шрифт</t>
+  </si>
+  <si>
+    <t>Шрифт тяжелочитабельный.</t>
+  </si>
+  <si>
+    <t>Все компоненты работают быстро</t>
+  </si>
+  <si>
+    <t>Интуитивность интерфейса</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Начальное окно удобное и интуитивное. Окно игры неудобное, недостаточно информации о проводимых действиях </t>
+  </si>
+  <si>
+    <t>Весь текст в программе соотвествует орфографическим нормам.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Положительно</t>
   </si>
 </sst>
 </file>
@@ -233,9 +257,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -245,7 +266,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -565,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60479AE-7537-4182-83BB-1AD5E14093DD}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,25 +619,25 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -619,250 +645,306 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>16</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>12</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>13</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="C25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>14</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>15</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>16</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A9:D9"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>